<commit_message>
Updated tasks file Added task 7 description
</commit_message>
<xml_diff>
--- a/deliverable3/tasks.xlsx
+++ b/deliverable3/tasks.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arman\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arman\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A5E0993-E650-40FE-BC73-F35B7EBF625E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{414CCDDF-D3DA-4E8F-B066-FFCF62F61DC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1905" yWindow="1905" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,9 +23,6 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>COMP 354</t>
-  </si>
-  <si>
-    <t>Task 7 Description:</t>
   </si>
   <si>
     <t>Task 8 Description:</t>
@@ -55,6 +52,9 @@
     <t>Task 1 Description: Calculate the multiplication of population standard deviation and 
 sample standard deviation of a set of values 
 (e.g., [10, 12, 23, 23, 16, 23, 21, 16]).</t>
+  </si>
+  <si>
+    <t>Task 7 Description: Calculate the multiplication of arccos(0.5) and arccos(-0.5) using the acos(x) Function ((acos(0.5)*acos(-0.5))</t>
   </si>
 </sst>
 </file>
@@ -950,8 +950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -977,7 +977,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -985,7 +985,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -999,52 +999,52 @@
     </row>
     <row r="6" spans="1:4" ht="52.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+    </row>
+    <row r="12" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="2"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-    </row>
-    <row r="12" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>1</v>
-      </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>